<commit_message>
chore: Update file paths and remove section from category
- Update file path for "设备接口_10_12" in xlsx_worklist
- Update file path for "设备接口-微电网参数" in csv_worklist
- Remove "传输线" section from "配电传输" category in microgrid_ports.json
</commit_message>
<xml_diff>
--- a/microgrid_base/设备信息库各参数_23_10_11_from_7_24.xlsx
+++ b/microgrid_base/设备信息库各参数_23_10_11_from_7_24.xlsx
@@ -2907,10 +2907,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -19572,7 +19572,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K733 A734 C734:K734 A735 C735:K735 A736:K736 A737 C737:K737 A738:K740 A741 C741:K741 A742:K1234" numberStoredAsText="1"/>
+    <ignoredError sqref="A742:K1234 C741:K741 A741 A738:K740 C737:K737 A737 A736:K736 C735:K735 A735 C734:K734 A734 A1:K733" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>